<commit_message>
Updated burnwound mapping to observation resource
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21607"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_B34CEF33A07BD798C8F294D8A859F1ED3923D6C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{27B5D8B5-0478-44A7-8326-24864CFCA368}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="DepthCodelist" sheetId="8" r:id="rId8"/>
     <sheet name="Terms of Use" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="188">
   <si>
     <t>Subject</t>
   </si>
@@ -301,9 +300,6 @@
     <t>SNOMED CT: 125666000 Brandwond</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>DateOfOnset</t>
   </si>
   <si>
@@ -323,9 +319,6 @@
   </si>
   <si>
     <t>Date on which the burn wound appeared.</t>
-  </si>
-  <si>
-    <t>Condition.onsetDateTime</t>
   </si>
   <si>
     <t>Extent</t>
@@ -344,12 +337,6 @@
 (Source: Brandwonden genezen. Hoe verder? [Healing Burn Wounds. What now?)</t>
   </si>
   <si>
-    <t>Condition.Extent (extension)</t>
-  </si>
-  <si>
-    <t>You could argue this is part of Condition.severity. Unfortunetaly Core does not allow slices in .severity. We chose Depth as the  concept for severity, since that has an Cardinality of 1.</t>
-  </si>
-  <si>
     <t>BrandwondSoort</t>
   </si>
   <si>
@@ -384,10 +371,6 @@
   </si>
   <si>
     <t>BurnWoundAnatomicalLocationCodelist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition.bodySite
-</t>
   </si>
   <si>
     <t>Laterality</t>
@@ -425,223 +408,248 @@
     <t>BurnWoundLateralityCodelist</t>
   </si>
   <si>
-    <t>Condition.bodySite.Laterality 
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>NL: Dieptegraad</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NL-CM:19.4.2</t>
+  </si>
+  <si>
+    <t>Description of the severity of the burn wound, ranging from degree 1 - 3.</t>
+  </si>
+  <si>
+    <t>SNOMED CT:116676008 Associated morphology</t>
+  </si>
+  <si>
+    <t>DepthCodelist</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>NL: Toelichting</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>NL-CM:19.4.5</t>
+  </si>
+  <si>
+    <t>Comment on the burn wound.</t>
+  </si>
+  <si>
+    <t>LOINC: 48767-8 Annotation comment</t>
+  </si>
+  <si>
+    <t>DateOfLastDressingChange</t>
+  </si>
+  <si>
+    <t>NL: DatumLaatsteVerbandwissel</t>
+  </si>
+  <si>
+    <t>NL-CM:19.4.8</t>
+  </si>
+  <si>
+    <t>Date on which the dressing was last changed.</t>
+  </si>
+  <si>
+    <t>extension is used also in pressureUlcer</t>
+  </si>
+  <si>
+    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.3</t>
+  </si>
+  <si>
+    <t>Conceptname</t>
+  </si>
+  <si>
+    <t>Conceptcode</t>
+  </si>
+  <si>
+    <t>Codesystem name</t>
+  </si>
+  <si>
+    <t>Codesystem OID</t>
+  </si>
+  <si>
+    <t>Chemical burn</t>
+  </si>
+  <si>
+    <t>26696002</t>
+  </si>
+  <si>
+    <t>SNOMED CT</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.6.96</t>
+  </si>
+  <si>
+    <t>Chemisch brandwond</t>
+  </si>
+  <si>
+    <t>Electrical burn</t>
+  </si>
+  <si>
+    <t>21720007</t>
+  </si>
+  <si>
+    <t>Elektrische brandwond</t>
+  </si>
+  <si>
+    <t>Thermal burn</t>
+  </si>
+  <si>
+    <t>105594005</t>
+  </si>
+  <si>
+    <t>Thermische brandwond</t>
+  </si>
+  <si>
+    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.2</t>
+  </si>
+  <si>
+    <t>SNOMED CT: &lt; 442083009 |Anatomical or acquired body structure|</t>
+  </si>
+  <si>
+    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.4</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>7771000</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>24028007</t>
+  </si>
+  <si>
+    <t>Rechts</t>
+  </si>
+  <si>
+    <t>Right and left</t>
+  </si>
+  <si>
+    <t>51440002</t>
+  </si>
+  <si>
+    <t>Rechts en links</t>
+  </si>
+  <si>
+    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.1</t>
+  </si>
+  <si>
+    <t>first degree burn injury</t>
+  </si>
+  <si>
+    <t>77140003</t>
+  </si>
+  <si>
+    <t>1e graad</t>
+  </si>
+  <si>
+    <t>superficial partial thickness burn</t>
+  </si>
+  <si>
+    <t>262587005</t>
+  </si>
+  <si>
+    <t>2e graad, oppervlakkig</t>
+  </si>
+  <si>
+    <t>deep partial thickness burn</t>
+  </si>
+  <si>
+    <t>262588000</t>
+  </si>
+  <si>
+    <t>2e graad, diep</t>
+  </si>
+  <si>
+    <t>third degree burn injury</t>
+  </si>
+  <si>
+    <t>80247002</t>
+  </si>
+  <si>
+    <t>3e graad</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>This Health and Care Information Model (a.k.a Clinical Building Block) has been made in collaboration with several different parties in healthcare. These parties asked Nictiz to manage good maintenance and development of the information models. Hereafter, these parties and Nictiz are referred to as the collaborating parties. The collaborating parties paid utmost attention to the reliability and topicality of the data in these Health and Care Information Models. Omissions and inaccuracies may however occur. The collaborating parties are not liable for any damages resulting from omissions or inaccuracies in the information provided, nor are they liable for damages resulting from problems caused by or inherent to distributing information on the internet, such as malfunctions, interruptions, errors or delays in information or services provide by the parties to you or by you to the parties via a website or via e-mail, or any other digital means. The collaborating parties will also not accept liability for any damages resulting from the use of data, advice or ideas provided by or on behalf of the parties by means of this Health and Care Information Model. The parties will not accept any liability for the content of information in this Health and Care Information Model to which or from which a hyperlink is referred. In the event of contradictions in mentioned Health and Care Information Model documents and files, the most recent and highest version of the listed order in the revisions will indicate the priority of the documents in question. If information included in the digital version of this Health and Care Information Model is also distributed in writing, the written version will be leading in case of textual differences. This will apply if both have the same version number and date. A definitive version has priority over a draft version. A revised version has priority over previous versions.</t>
+  </si>
+  <si>
+    <t>Terms of Use</t>
+  </si>
+  <si>
+    <t>The user may use the information in this Health and Care Information Model without limitations. The copyright provisions in the paragraph concerned apply to copying, distributing and passing on information from this Health and Care Information Model.</t>
+  </si>
+  <si>
+    <t>Copyrights</t>
+  </si>
+  <si>
+    <t>The user may copy, distribute and pass on the information in this Health and Care Information Model under the conditions that apply for Creative Commons license Attribution-NonCommercial-ShareAlike 3.0 Netherlands (CC BY-NCSA-3.0). The content is available under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 (see also http://creativecommons.org/licenses/by-nc-sa/3.0/nl/)</t>
+  </si>
+  <si>
+    <t>.component.onsetDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.bodySite
+</t>
+  </si>
+  <si>
+    <t>.bodySite.laterality 
 (extension, reference to BodySite Qualifier)</t>
   </si>
   <si>
-    <t>Depth</t>
-  </si>
-  <si>
-    <t>NL: Dieptegraad</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>NL-CM:19.4.2</t>
-  </si>
-  <si>
-    <t>Description of the severity of the burn wound, ranging from degree 1 - 3.</t>
-  </si>
-  <si>
-    <t>SNOMED CT:116676008 Associated morphology</t>
-  </si>
-  <si>
-    <t>DepthCodelist</t>
-  </si>
-  <si>
-    <t>Condition.grade.summary</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>NL: Toelichting</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>NL-CM:19.4.5</t>
-  </si>
-  <si>
-    <t>Comment on the burn wound.</t>
-  </si>
-  <si>
-    <t>LOINC: 48767-8 Annotation comment</t>
-  </si>
-  <si>
-    <t>Condition.note</t>
-  </si>
-  <si>
-    <t>DateOfLastDressingChange</t>
-  </si>
-  <si>
-    <t>NL: DatumLaatsteVerbandwissel</t>
-  </si>
-  <si>
-    <t>NL-CM:19.4.8</t>
-  </si>
-  <si>
-    <t>Date on which the dressing was last changed.</t>
-  </si>
-  <si>
-    <t>Condition.dateOfLastDressingChange
-(extension)</t>
-  </si>
-  <si>
-    <t>extension is used also in pressureUlcer</t>
-  </si>
-  <si>
-    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.3</t>
-  </si>
-  <si>
-    <t>Conceptname</t>
-  </si>
-  <si>
-    <t>Conceptcode</t>
-  </si>
-  <si>
-    <t>Codesystem name</t>
-  </si>
-  <si>
-    <t>Codesystem OID</t>
-  </si>
-  <si>
-    <t>Chemical burn</t>
-  </si>
-  <si>
-    <t>26696002</t>
-  </si>
-  <si>
-    <t>SNOMED CT</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.6.96</t>
-  </si>
-  <si>
-    <t>Chemisch brandwond</t>
-  </si>
-  <si>
-    <t>Electrical burn</t>
-  </si>
-  <si>
-    <t>21720007</t>
-  </si>
-  <si>
-    <t>Elektrische brandwond</t>
-  </si>
-  <si>
-    <t>Thermal burn</t>
-  </si>
-  <si>
-    <t>105594005</t>
-  </si>
-  <si>
-    <t>Thermische brandwond</t>
-  </si>
-  <si>
-    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.2</t>
-  </si>
-  <si>
-    <t>SNOMED CT: &lt; 442083009 |Anatomical or acquired body structure|</t>
-  </si>
-  <si>
-    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.4</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>7771000</t>
-  </si>
-  <si>
-    <t>Links</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>24028007</t>
-  </si>
-  <si>
-    <t>Rechts</t>
-  </si>
-  <si>
-    <t>Right and left</t>
-  </si>
-  <si>
-    <t>51440002</t>
-  </si>
-  <si>
-    <t>Rechts en links</t>
-  </si>
-  <si>
-    <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.1</t>
-  </si>
-  <si>
-    <t>first degree burn injury</t>
-  </si>
-  <si>
-    <t>77140003</t>
-  </si>
-  <si>
-    <t>1e graad</t>
-  </si>
-  <si>
-    <t>superficial partial thickness burn</t>
-  </si>
-  <si>
-    <t>262587005</t>
-  </si>
-  <si>
-    <t>2e graad, oppervlakkig</t>
-  </si>
-  <si>
-    <t>deep partial thickness burn</t>
-  </si>
-  <si>
-    <t>262588000</t>
-  </si>
-  <si>
-    <t>2e graad, diep</t>
-  </si>
-  <si>
-    <t>third degree burn injury</t>
-  </si>
-  <si>
-    <t>80247002</t>
-  </si>
-  <si>
-    <t>3e graad</t>
-  </si>
-  <si>
-    <t>Disclaimer</t>
-  </si>
-  <si>
-    <t>This Health and Care Information Model (a.k.a Clinical Building Block) has been made in collaboration with several different parties in healthcare. These parties asked Nictiz to manage good maintenance and development of the information models. Hereafter, these parties and Nictiz are referred to as the collaborating parties. The collaborating parties paid utmost attention to the reliability and topicality of the data in these Health and Care Information Models. Omissions and inaccuracies may however occur. The collaborating parties are not liable for any damages resulting from omissions or inaccuracies in the information provided, nor are they liable for damages resulting from problems caused by or inherent to distributing information on the internet, such as malfunctions, interruptions, errors or delays in information or services provide by the parties to you or by you to the parties via a website or via e-mail, or any other digital means. The collaborating parties will also not accept liability for any damages resulting from the use of data, advice or ideas provided by or on behalf of the parties by means of this Health and Care Information Model. The parties will not accept any liability for the content of information in this Health and Care Information Model to which or from which a hyperlink is referred. In the event of contradictions in mentioned Health and Care Information Model documents and files, the most recent and highest version of the listed order in the revisions will indicate the priority of the documents in question. If information included in the digital version of this Health and Care Information Model is also distributed in writing, the written version will be leading in case of textual differences. This will apply if both have the same version number and date. A definitive version has priority over a draft version. A revised version has priority over previous versions.</t>
-  </si>
-  <si>
-    <t>Terms of Use</t>
-  </si>
-  <si>
-    <t>The user may use the information in this Health and Care Information Model without limitations. The copyright provisions in the paragraph concerned apply to copying, distributing and passing on information from this Health and Care Information Model.</t>
-  </si>
-  <si>
-    <t>Copyrights</t>
-  </si>
-  <si>
-    <t>The user may copy, distribute and pass on the information in this Health and Care Information Model under the conditions that apply for Creative Commons license Attribution-NonCommercial-ShareAlike 3.0 Netherlands (CC BY-NCSA-3.0). The content is available under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 (see also http://creativecommons.org/licenses/by-nc-sa/3.0/nl/)</t>
+    <t>Observation.code</t>
+  </si>
+  <si>
+    <t>.component.burnType.Value</t>
+  </si>
+  <si>
+    <t>.component.extent (extension, valueCodeableConcept)</t>
+  </si>
+  <si>
+    <t>.component.depth (valueCodeableConcept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">component.dateOfLastDressingChange (valuedatetime)
+</t>
+  </si>
+  <si>
+    <t>The model of this HCIM serves a purpose as a snapshot of the injury, this is why we chose Observation over Condition</t>
+  </si>
+  <si>
+    <t>.woundPhoto (extension, binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wil be added later in the HCIM. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -683,6 +691,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -774,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -827,9 +841,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -859,7 +876,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -900,7 +917,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -941,7 +958,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1015,7 +1032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1048,26 +1065,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1100,23 +1100,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1292,10 +1275,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1419,7 +1402,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1430,10 +1413,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1639,10 +1622,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
@@ -1656,11 +1639,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:R11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1673,7 +1656,9 @@
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="17" width="30" customWidth="1"/>
+    <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="16" max="16" width="33.85546875" customWidth="1"/>
+    <col min="17" max="17" width="30" customWidth="1"/>
     <col min="18" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1720,7 +1705,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="25.5">
+    <row r="3" spans="2:18" ht="51">
       <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
@@ -1748,42 +1733,44 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="14" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1791,110 +1778,110 @@
     <row r="5" spans="2:18" ht="127.5">
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
       <c r="H5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="M5" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>95</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="Q5" s="14"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
       <c r="H6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="P6" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>180</v>
+      </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="2:18" ht="25.5">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
       <c r="H7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="P7" s="14" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="1"/>
@@ -1902,38 +1889,38 @@
     <row r="8" spans="2:18" ht="38.25">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="1"/>
@@ -1941,38 +1928,38 @@
     <row r="9" spans="2:18" ht="25.5">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
       <c r="H9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="P9" s="14" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="1"/>
@@ -1980,83 +1967,106 @@
     <row r="10" spans="2:18" ht="25.5">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
       <c r="H10" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="14" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="2:18" ht="38.25">
+    <row r="11" spans="2:18">
       <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
-        <v>132</v>
-      </c>
+      <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>137</v>
+        <v>186</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="2:18" ht="38.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O6" location="BurnTypeCodelist!A1" display="BurnTypeCodelist" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="O7" location="BurnWoundAnatomicalLocationCode!A1" display="BurnWoundAnatomicalLocationCodelist" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="O8" location="BurnWoundLateralityCodelist!A1" display="BurnWoundLateralityCodelist" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="O9" location="DepthCodelist!A1" display="DepthCodelist" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="O6" location="BurnTypeCodelist!A1" display="BurnTypeCodelist"/>
+    <hyperlink ref="O7" location="BurnWoundAnatomicalLocationCode!A1" display="BurnWoundAnatomicalLocationCodelist"/>
+    <hyperlink ref="O8" location="BurnWoundLateralityCodelist!A1" display="BurnWoundLateralityCodelist"/>
+    <hyperlink ref="O9" location="DepthCodelist!A1" display="DepthCodelist"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2067,10 +2077,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2083,27 +2093,27 @@
   <sheetData>
     <row r="3" spans="3:7">
       <c r="C3" s="17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
@@ -2111,53 +2121,53 @@
     </row>
     <row r="5" spans="3:7">
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2173,10 +2183,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2189,33 +2199,33 @@
   <sheetData>
     <row r="3" spans="3:5">
       <c r="C3" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="3:5">
       <c r="C4" s="13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="38.25">
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2231,10 +2241,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2247,27 +2257,27 @@
   <sheetData>
     <row r="3" spans="3:7">
       <c r="C3" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
@@ -2275,53 +2285,53 @@
     </row>
     <row r="5" spans="3:7">
       <c r="C5" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2337,10 +2347,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2353,27 +2363,27 @@
   <sheetData>
     <row r="3" spans="3:7">
       <c r="C3" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
@@ -2381,70 +2391,70 @@
     </row>
     <row r="5" spans="3:7">
       <c r="C5" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="3:7">
       <c r="C8" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2460,10 +2470,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2472,32 +2482,32 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="16" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="140.25">
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="16" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="25.5">
       <c r="B5" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="16" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="38.25">
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2697,6 +2707,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2705,20 +2721,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update and added mappings
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -639,10 +639,10 @@
     <t>The model of this HCIM serves a purpose as a snapshot of the injury, this is why we chose Observation over Condition</t>
   </si>
   <si>
-    <t>.woundPhoto (extension, binary)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wil be added later in the HCIM. </t>
+  </si>
+  <si>
+    <t>.woundImage (extension, binary)</t>
   </si>
 </sst>
 </file>
@@ -838,10 +838,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -876,7 +876,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -917,7 +917,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -958,7 +958,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1427,10 +1427,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
@@ -1642,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1735,7 +1735,7 @@
       <c r="P3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="17" t="s">
         <v>185</v>
       </c>
       <c r="R3" s="3"/>
@@ -2017,10 +2017,10 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q11" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="R11" s="1"/>
     </row>
@@ -2092,15 +2092,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
@@ -2198,11 +2198,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2256,15 +2256,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
@@ -2362,15 +2362,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="13" t="s">
@@ -2707,18 +2707,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2741,18 +2741,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Some minor tweaks to recent mappings
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E623760B-517D-4AAA-9C2F-80C33AC16235}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" activeTab="3"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,14 +25,6 @@
     <sheet name="Terms of Use" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -391,6 +389,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>e.g.</t>
     </r>
@@ -398,6 +397,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> left</t>
     </r>
@@ -463,9 +463,6 @@
     <t>Date on which the dressing was last changed.</t>
   </si>
   <si>
-    <t>extension is used also in pressureUlcer</t>
-  </si>
-  <si>
     <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.3</t>
   </si>
   <si>
@@ -621,9 +618,6 @@
     <t>Observation.code</t>
   </si>
   <si>
-    <t>.component.extent (extension, valueCodeableConcept)</t>
-  </si>
-  <si>
     <t xml:space="preserve">.comment </t>
   </si>
   <si>
@@ -643,9 +637,6 @@
     <t xml:space="preserve">Valueset </t>
   </si>
   <si>
-    <t>.component.burnType.ValueCodableconcept</t>
-  </si>
-  <si>
     <t>.valueCodeableConcept</t>
   </si>
   <si>
@@ -698,13 +689,22 @@
   </si>
   <si>
     <t>Burn, thermal wound, burn wound</t>
+  </si>
+  <si>
+    <t>Not on .effective, as that refers to the dt at which the observation was done</t>
+  </si>
+  <si>
+    <t>.component.burnType (ValueCodableconcept)</t>
+  </si>
+  <si>
+    <t>.component.extent (valueQuantity)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -714,28 +714,33 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -905,18 +910,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1066,7 +1071,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1107,7 +1112,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1148,7 +1153,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1203,11 +1208,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10241"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1215,6 +1223,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1244,11 +1275,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10242"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1256,6 +1290,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1285,11 +1342,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10243"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1297,6 +1357,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1326,11 +1409,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10244"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1338,6 +1424,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1367,11 +1476,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10245"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1379,6 +1491,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1408,11 +1543,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10246"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1420,6 +1558,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1449,11 +1610,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10247"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1461,6 +1625,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1490,11 +1677,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10248"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1502,6 +1692,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1531,11 +1744,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10249"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1543,6 +1759,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1572,11 +1811,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10250"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1584,6 +1826,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1613,11 +1878,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10251"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1625,6 +1893,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1654,11 +1945,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10252"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1666,6 +1960,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1695,11 +2012,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10253"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1707,6 +2027,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1736,11 +2079,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10254"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1748,6 +2094,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1777,11 +2146,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10255"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1789,6 +2161,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1818,11 +2213,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10256"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1830,6 +2228,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1859,11 +2280,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10257"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1871,6 +2295,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1900,11 +2347,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10258"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1912,6 +2362,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1941,11 +2414,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10259"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1953,6 +2429,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1982,11 +2481,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10260"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1994,6 +2496,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2023,11 +2548,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10261"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2035,6 +2563,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2064,11 +2615,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10262"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2076,6 +2630,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2105,11 +2682,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10263"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2117,6 +2697,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2146,11 +2749,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10264"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000018280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2158,6 +2764,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2187,11 +2816,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10265"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2199,6 +2831,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2228,11 +2883,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10266"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2240,6 +2898,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2269,11 +2950,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10267"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2281,6 +2965,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2310,11 +3017,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10268"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2322,6 +3032,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2351,11 +3084,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10269"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2363,6 +3099,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2392,11 +3151,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10270"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E280000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2404,6 +3166,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2415,7 +3200,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2457,7 +3242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2490,9 +3275,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2525,6 +3327,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2700,20 +3519,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2729,7 +3548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2737,7 +3556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2745,7 +3564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2753,7 +3572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2761,7 +3580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2769,7 +3588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2777,7 +3596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +3604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2793,7 +3612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="89.25">
+    <row r="12" spans="2:3" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2801,7 +3620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2809,7 +3628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="395.25">
+    <row r="14" spans="2:3" ht="395.25" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2817,7 +3636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51">
+    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
@@ -2827,7 +3646,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2838,44 +3657,44 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="16" t="s">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="16" t="s">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="38.25">
-      <c r="B7" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2884,26 +3703,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="19"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2911,7 +3730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2919,7 +3738,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
@@ -2927,7 +3746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
@@ -2935,7 +3754,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +3762,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -2951,13 +3770,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
@@ -2965,13 +3784,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2979,13 +3798,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2993,7 +3812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
@@ -3001,7 +3820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -3009,7 +3828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -3017,7 +3836,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -3025,7 +3844,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
@@ -3033,7 +3852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3041,7 +3860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -3049,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3057,7 +3876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>58</v>
       </c>
@@ -3065,7 +3884,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
@@ -3073,7 +3892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
@@ -3093,14 +3912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
@@ -3110,113 +3929,113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C2" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D3" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="O1" s="20"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="21" t="s">
+      <c r="D4" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="21" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="21" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="21" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="21" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="21" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="22" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="21" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="21"/>
+      <c r="D10" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>201</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="C10" s="22"/>
-      <c r="D10" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="21" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3893,14 +4712,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3916,7 +4735,7 @@
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3953,10 +4772,10 @@
         <v>71</v>
       </c>
       <c r="Q2" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>184</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>186</v>
       </c>
       <c r="S2" s="15" t="s">
         <v>72</v>
@@ -3965,7 +4784,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="51">
+    <row r="3" spans="2:20" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
@@ -3993,16 +4812,16 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>80</v>
@@ -4032,16 +4851,18 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R4" s="14"/>
-      <c r="S4" s="1"/>
+      <c r="S4" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="2:20" ht="127.5">
+    <row r="5" spans="2:20" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
         <v>87</v>
@@ -4071,16 +4892,16 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="14" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="2:20" ht="25.5">
+    <row r="6" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>92</v>
@@ -4112,10 +4933,10 @@
         <v>97</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>2</v>
@@ -4123,7 +4944,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="2:20" ht="25.5">
+    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
         <v>98</v>
@@ -4157,10 +4978,10 @@
         <v>103</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R7" s="14" t="s">
         <v>2</v>
@@ -4168,7 +4989,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="2:20" ht="38.25">
+    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
         <v>104</v>
@@ -4202,10 +5023,10 @@
         <v>109</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R8" s="14" t="s">
         <v>2</v>
@@ -4213,7 +5034,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25">
+    <row r="9" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
         <v>110</v>
@@ -4247,20 +5068,20 @@
         <v>117</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
         <v>118</v>
@@ -4292,16 +5113,16 @@
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="2:20" ht="38.25">
+    <row r="11" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
         <v>124</v>
@@ -4331,23 +5152,21 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R11" s="14"/>
-      <c r="S11" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O6" location="BurnTypeCodelist!A1" display="BurnTypeCodelist"/>
-    <hyperlink ref="O7" location="BurnWoundAnatomicalLocationCode!A1" display="BurnWoundAnatomicalLocationCodelist"/>
-    <hyperlink ref="O8" location="BurnWoundLateralityCodelist!A1" display="BurnWoundLateralityCodelist"/>
-    <hyperlink ref="O9" location="DepthCodelist!A1" display="DepthCodelist"/>
+    <hyperlink ref="O6" location="BurnTypeCodelist!A1" display="BurnTypeCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="O7" location="BurnWoundAnatomicalLocationCode!A1" display="BurnWoundAnatomicalLocationCodelist" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O8" location="BurnWoundLateralityCodelist!A1" display="BurnWoundLateralityCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O9" location="DepthCodelist!A1" display="DepthCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4358,12 +5177,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4372,83 +5191,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4464,49 +5283,49 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="3:5">
-      <c r="C4" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="38.25">
-      <c r="C5" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4522,12 +5341,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4536,83 +5355,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4628,12 +5447,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4642,100 +5461,100 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="25.5">
-      <c r="C6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="1" t="s">
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4751,6 +5570,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4941,22 +5775,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4973,21 +5809,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add: work in progress profiling BurnWound
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -609,9 +609,6 @@
 (extension, reference to BodySite Qualifier)</t>
   </si>
   <si>
-    <t>Observation.code</t>
-  </si>
-  <si>
     <t xml:space="preserve">.comment </t>
   </si>
   <si>
@@ -692,6 +689,9 @@
   </si>
   <si>
     <t>.component.extent (valueQuantity)</t>
+  </si>
+  <si>
+    <t>Condition.code (derived from zib-problem)</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1065,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1106,7 +1106,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1147,7 +1147,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2702,7 +2702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2887,7 +2887,7 @@
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3095,7 +3095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3125,19 +3125,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>190</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>191</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
@@ -3146,76 +3146,76 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C10" s="21"/>
       <c r="D10" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3895,8 +3895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3952,10 +3952,10 @@
         <v>71</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S2" s="15" t="s">
         <v>72</v>
@@ -3992,12 +3992,12 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T3" s="3"/>
     </row>
@@ -4034,11 +4034,11 @@
         <v>175</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R4" s="14"/>
       <c r="S4" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T4" s="1"/>
     </row>
@@ -4072,10 +4072,10 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
@@ -4113,10 +4113,10 @@
         <v>97</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>2</v>
@@ -4161,7 +4161,7 @@
         <v>176</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R7" s="14" t="s">
         <v>2</v>
@@ -4206,7 +4206,7 @@
         <v>177</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R8" s="14" t="s">
         <v>2</v>
@@ -4248,16 +4248,16 @@
         <v>117</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T9" s="1"/>
     </row>
@@ -4293,10 +4293,10 @@
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="1"/>
@@ -4332,10 +4332,10 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="1"/>
@@ -4750,6 +4750,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4940,22 +4955,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4972,21 +4989,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: changed mapping for wound and skin disorder profiles
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
   <si>
     <t>Subject</t>
   </si>
@@ -598,9 +598,6 @@
     <t>The user may copy, distribute and pass on the information in this Health and Care Information Model under the conditions that apply for Creative Commons license Attribution-NonCommercial-ShareAlike 3.0 Netherlands (CC BY-NCSA-3.0). The content is available under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 (see also http://creativecommons.org/licenses/by-nc-sa/3.0/nl/)</t>
   </si>
   <si>
-    <t>.component.onsetDateTime</t>
-  </si>
-  <si>
     <t xml:space="preserve">.bodySite
 </t>
   </si>
@@ -609,89 +606,83 @@
 (extension, reference to BodySite Qualifier)</t>
   </si>
   <si>
-    <t>Observation.code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.comment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">component.dateOfLastDressingChange (valuedatetime)
+    <t>equivalence</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valueset </t>
+  </si>
+  <si>
+    <t>Checkbox searched for existing profiles / implementation on:</t>
+  </si>
+  <si>
+    <t>Checkbox!</t>
+  </si>
+  <si>
+    <t>Searchwords</t>
+  </si>
+  <si>
+    <t>Found results:</t>
+  </si>
+  <si>
+    <t>Relevance:</t>
+  </si>
+  <si>
+    <t>HL7 FHIR Specification</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles - latest version latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry - latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
+  </si>
+  <si>
+    <t>Simplifier.net</t>
+  </si>
+  <si>
+    <t>Zulip (chat.fhir.org)</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>Burn, thermal wound, burn wound</t>
+  </si>
+  <si>
+    <t>.onsetDateTime</t>
+  </si>
+  <si>
+    <t>Condition.category</t>
+  </si>
+  <si>
+    <t>.extent (extension, valueQuantity)</t>
+  </si>
+  <si>
+    <t>.code(ValueCodableconcept)</t>
+  </si>
+  <si>
+    <t>.stage.summary</t>
+  </si>
+  <si>
+    <t>.note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.dateOfLastDressingChange (extension, valueDatetime)
 </t>
-  </si>
-  <si>
-    <t>The model of this HCIM serves a purpose as a snapshot of the injury, this is why we chose Observation over Condition</t>
-  </si>
-  <si>
-    <t>equivalence</t>
-  </si>
-  <si>
-    <t>equal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valueset </t>
-  </si>
-  <si>
-    <t>.valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Is required, therefor the main value for the HCIM, this is why we chose this as our observation.value[x]</t>
-  </si>
-  <si>
-    <t>Checkbox searched for existing profiles / implementation on:</t>
-  </si>
-  <si>
-    <t>Checkbox!</t>
-  </si>
-  <si>
-    <t>Searchwords</t>
-  </si>
-  <si>
-    <t>Found results:</t>
-  </si>
-  <si>
-    <t>Relevance:</t>
-  </si>
-  <si>
-    <t>HL7 FHIR Specification</t>
-  </si>
-  <si>
-    <t>HL7 FHIR profiles</t>
-  </si>
-  <si>
-    <t>HL7 FHIR profiles - latest version latest version (build)</t>
-  </si>
-  <si>
-    <t>HL7 FHIR extension registry</t>
-  </si>
-  <si>
-    <t>HL7 FHIR extension registry - latest version (build)</t>
-  </si>
-  <si>
-    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
-  </si>
-  <si>
-    <t>Simplifier.net</t>
-  </si>
-  <si>
-    <t>Zulip (chat.fhir.org)</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google </t>
-  </si>
-  <si>
-    <t>Burn, thermal wound, burn wound</t>
-  </si>
-  <si>
-    <t>Not on .effective, as that refers to the dt at which the observation was done</t>
-  </si>
-  <si>
-    <t>.component.burnType (ValueCodableconcept)</t>
-  </si>
-  <si>
-    <t>.component.extent (valueQuantity)</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1056,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1106,7 +1097,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1147,7 +1138,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3125,19 +3116,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
@@ -3146,76 +3137,76 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>193</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C10" s="21"/>
       <c r="D10" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3896,7 +3887,7 @@
   <dimension ref="B2:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3952,10 +3943,10 @@
         <v>71</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="S2" s="15" t="s">
         <v>72</v>
@@ -3964,7 +3955,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
@@ -3992,16 +3983,14 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="17" t="s">
-        <v>181</v>
-      </c>
+      <c r="S3" s="17"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>80</v>
@@ -4031,15 +4020,13 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="14" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R4" s="14"/>
-      <c r="S4" s="14" t="s">
-        <v>203</v>
-      </c>
+      <c r="S4" s="14"/>
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="2:20" ht="127.5" x14ac:dyDescent="0.2">
@@ -4072,16 +4059,16 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="14" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>92</v>
@@ -4113,10 +4100,10 @@
         <v>97</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>2</v>
@@ -4158,10 +4145,10 @@
         <v>103</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R7" s="14" t="s">
         <v>2</v>
@@ -4203,10 +4190,10 @@
         <v>109</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R8" s="14" t="s">
         <v>2</v>
@@ -4214,7 +4201,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
         <v>110</v>
@@ -4248,17 +4235,15 @@
         <v>117</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="S9" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="S9" s="14"/>
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
@@ -4293,10 +4278,10 @@
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="14" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="1"/>
@@ -4332,10 +4317,10 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="1"/>
@@ -4750,6 +4735,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4940,22 +4940,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4972,21 +4974,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
wip: profile and extension zib-burnwound. ToDo: add example
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" activeTab="4"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1056,7 +1056,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1097,7 +1097,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1138,7 +1138,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3086,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3886,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4345,7 +4345,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4509,7 +4511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4615,7 +4619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4735,21 +4741,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4940,24 +4931,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4974,4 +4963,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
done: zib-BurnWound profile, extensions and example
to be reviewed
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -681,7 +681,7 @@
     <t>.note</t>
   </si>
   <si>
-    <t xml:space="preserve">.dateOfLastDressingChange (extension, valueDatetime)
+    <t xml:space="preserve">.dateOfLastDressingChange (extension, valueDate)
 </t>
   </si>
 </sst>
@@ -1056,7 +1056,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1097,7 +1097,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1138,7 +1138,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3886,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4741,6 +4741,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4931,22 +4946,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4963,21 +4980,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Draft profiles from the defunct "develop" branch
</commit_message>
<xml_diff>
--- a/Mappings/Burnwound - STU3.xlsx
+++ b/Mappings/Burnwound - STU3.xlsx
@@ -4,33 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="270" yWindow="540" windowWidth="20775" windowHeight="7365" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
-    <sheet name="BurnTypeCodelist" sheetId="5" r:id="rId5"/>
-    <sheet name="BurnWoundAnatomicalLocationCode" sheetId="6" r:id="rId6"/>
-    <sheet name="BurnWoundLateralityCodelist" sheetId="7" r:id="rId7"/>
-    <sheet name="DepthCodelist" sheetId="8" r:id="rId8"/>
-    <sheet name="Terms of Use" sheetId="9" r:id="rId9"/>
+    <sheet name="Research" sheetId="10" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
+    <sheet name="BurnTypeCodelist" sheetId="5" r:id="rId6"/>
+    <sheet name="BurnWoundAnatomicalLocationCode" sheetId="6" r:id="rId7"/>
+    <sheet name="BurnWoundLateralityCodelist" sheetId="7" r:id="rId8"/>
+    <sheet name="DepthCodelist" sheetId="8" r:id="rId9"/>
+    <sheet name="Terms of Use" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
   <si>
     <t>Subject</t>
   </si>
@@ -390,6 +383,7 @@
         <i/>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>e.g.</t>
     </r>
@@ -397,6 +391,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> left</t>
     </r>
@@ -462,9 +457,6 @@
     <t>Date on which the dressing was last changed.</t>
   </si>
   <si>
-    <t>extension is used also in pressureUlcer</t>
-  </si>
-  <si>
     <t>Valueset OID: 2.16.840.1.113883.2.4.3.11.60.40.2.19.4.3</t>
   </si>
   <si>
@@ -604,9 +596,6 @@
   </si>
   <si>
     <t>The user may copy, distribute and pass on the information in this Health and Care Information Model under the conditions that apply for Creative Commons license Attribution-NonCommercial-ShareAlike 3.0 Netherlands (CC BY-NCSA-3.0). The content is available under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 (see also http://creativecommons.org/licenses/by-nc-sa/3.0/nl/)</t>
-  </si>
-  <si>
-    <t>.component.onsetDateTime</t>
   </si>
   <si>
     <t xml:space="preserve">.bodySite
@@ -617,39 +606,90 @@
 (extension, reference to BodySite Qualifier)</t>
   </si>
   <si>
-    <t>Observation.code</t>
-  </si>
-  <si>
-    <t>.component.burnType.Value</t>
-  </si>
-  <si>
-    <t>.component.extent (extension, valueCodeableConcept)</t>
-  </si>
-  <si>
-    <t>.component.depth (valueCodeableConcept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.comment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">component.dateOfLastDressingChange (valuedatetime)
+    <t>equivalence</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valueset </t>
+  </si>
+  <si>
+    <t>Checkbox searched for existing profiles / implementation on:</t>
+  </si>
+  <si>
+    <t>Checkbox!</t>
+  </si>
+  <si>
+    <t>Searchwords</t>
+  </si>
+  <si>
+    <t>Found results:</t>
+  </si>
+  <si>
+    <t>Relevance:</t>
+  </si>
+  <si>
+    <t>HL7 FHIR Specification</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles - latest version latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry - latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
+  </si>
+  <si>
+    <t>Simplifier.net</t>
+  </si>
+  <si>
+    <t>Zulip (chat.fhir.org)</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>Burn, thermal wound, burn wound</t>
+  </si>
+  <si>
+    <t>.onsetDateTime</t>
+  </si>
+  <si>
+    <t>Condition.category</t>
+  </si>
+  <si>
+    <t>.extent (extension, valueQuantity)</t>
+  </si>
+  <si>
+    <t>.code(ValueCodableconcept)</t>
+  </si>
+  <si>
+    <t>.stage.summary</t>
+  </si>
+  <si>
+    <t>.note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.dateOfLastDressingChange (extension, valueDate)
 </t>
-  </si>
-  <si>
-    <t>The model of this HCIM serves a purpose as a snapshot of the injury, this is why we chose Observation over Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wil be added later in the HCIM. </t>
-  </si>
-  <si>
-    <t>.woundImage (extension, binary)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -659,28 +699,33 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -697,6 +742,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -788,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -844,6 +895,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,6 +919,126 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -951,7 +1131,7 @@
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="635000" y="635000"/>
+    <xdr:pos x="606425" y="635000"/>
     <xdr:ext cx="8191500" cy="5286375"/>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -975,7 +1155,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="606425" y="635000"/>
           <a:ext cx="8191500" cy="5286375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -986,6 +1166,1241 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10241" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10241"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10242" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10242"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10243" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10243"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10244" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10244"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10245" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10245"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10246" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10246"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10247" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10247"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10248" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10248"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10249" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10249"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10250" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10250"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10251" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10251"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10252" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10252"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10253" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10253"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10254" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10254"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10255" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10255"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10256" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10256"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10257" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10257"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10258" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10258"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10259" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10259"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10260" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10260"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10261" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10261"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10262" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10262"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10263" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10263"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10264" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10264"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10265" name="Check Box 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10265"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10266" name="Check Box 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10266"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10267" name="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10267"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10268" name="Check Box 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10268"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10269" name="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10269"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10270" name="Check Box 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s10270"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1282,13 +2697,13 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +2719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1328,7 +2743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1336,7 +2751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +2759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1352,7 +2767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1360,7 +2775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +2783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="89.25">
+    <row r="12" spans="2:3" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1376,7 +2791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1384,7 +2799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="395.25">
+    <row r="14" spans="2:3" ht="395.25" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1392,7 +2807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51">
+    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1412,6 +2827,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="150" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
@@ -1420,19 +2881,19 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1440,7 +2901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1448,7 +2909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1456,7 +2917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1464,7 +2925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1472,7 +2933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1480,13 +2941,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1494,13 +2955,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1508,13 +2969,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1522,7 +2983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1530,7 +2991,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1538,7 +2999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1546,7 +3007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1554,7 +3015,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>53</v>
       </c>
@@ -1562,7 +3023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
@@ -1570,7 +3031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1578,7 +3039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
@@ -1586,7 +3047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>58</v>
       </c>
@@ -1594,7 +3055,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1602,7 +3063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
@@ -1625,11 +3086,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
@@ -1639,14 +3100,797 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="21"/>
+      <c r="D10" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10241" r:id="rId3" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10242" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10243" r:id="rId5" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10244" r:id="rId6" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10245" r:id="rId7" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10246" r:id="rId8" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10247" r:id="rId9" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10248" r:id="rId10" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10249" r:id="rId11" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10250" r:id="rId12" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10251" r:id="rId13" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10252" r:id="rId14" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10253" r:id="rId15" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10254" r:id="rId16" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10255" r:id="rId17" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10256" r:id="rId18" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10257" r:id="rId19" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10258" r:id="rId20" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10259" r:id="rId21" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10260" r:id="rId22" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10261" r:id="rId23" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10262" r:id="rId24" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10263" r:id="rId25" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10264" r:id="rId26" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10265" r:id="rId27" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10266" r:id="rId28" name="Check Box 26">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10267" r:id="rId29" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10268" r:id="rId30" name="Check Box 28">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10269" r:id="rId31" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="10270" r:id="rId32" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R12"/>
+  <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -1657,12 +3901,12 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="33.85546875" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="16" max="18" width="33.85546875" customWidth="1"/>
+    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1698,14 +3942,20 @@
       <c r="P2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="51">
+    <row r="3" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>74</v>
       </c>
@@ -1733,14 +3983,14 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>185</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="2:18">
+      <c r="S3" s="17"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>80</v>
@@ -1770,12 +4020,16 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="2:18" ht="127.5">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
         <v>87</v>
@@ -1805,12 +4059,16 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="2:18">
+        <v>198</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>92</v>
@@ -1842,12 +4100,18 @@
         <v>97</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="2:18" ht="25.5">
+        <v>199</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
         <v>98</v>
@@ -1881,12 +4145,18 @@
         <v>103</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="2:18" ht="38.25">
+        <v>175</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
         <v>104</v>
@@ -1920,12 +4190,18 @@
         <v>109</v>
       </c>
       <c r="P8" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q8" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="2:18" ht="25.5">
+      <c r="R8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
         <v>110</v>
@@ -1959,12 +4235,18 @@
         <v>117</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="2:18" ht="25.5">
+        <v>200</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="14"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
         <v>118</v>
@@ -1996,70 +4278,53 @@
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="2:18">
+        <v>201</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="R10" s="14"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="14" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="2:18" ht="38.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R12" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="R11" s="14"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2076,13 +4341,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2091,83 +4358,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2182,7 +4449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E5"/>
   <sheetViews>
@@ -2190,42 +4457,42 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="3:5">
-      <c r="C4" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="38.25">
-      <c r="C5" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2240,13 +4507,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2255,83 +4524,83 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2346,13 +4615,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2361,100 +4632,100 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="25.5">
-      <c r="C6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="1" t="s">
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2469,53 +4740,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="2" max="2" width="150" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="16" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="140.25">
-      <c r="B3" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="25.5">
-      <c r="B5" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="38.25">
-      <c r="B7" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -2706,22 +4946,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBF3DAC-BFFB-4187-A170-7CCBD50B0557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2738,21 +4980,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28504DDE-B48C-416D-B4D5-C4C094753D8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB09C7B-290D-4D11-9651-C89CB11FA5C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>